<commit_message>
attempting 2019 d 11 p1
</commit_message>
<xml_diff>
--- a/Tracking Sheet.xlsx
+++ b/Tracking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AOCv3\AOC-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181F804F-61BB-476A-B453-DD62A4BAA1FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D58A814-AA8F-4939-8FB8-E1AEC2270A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1004,10 +1004,10 @@
         <v>2</v>
       </c>
       <c r="K7" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L7" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M7" s="8">
         <v>0</v>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="AC7" s="10">
         <f t="shared" si="0"/>
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.55000000000000004">
@@ -1067,7 +1067,7 @@
     <row r="10" spans="1:32" x14ac:dyDescent="0.55000000000000004">
       <c r="AC10" s="10">
         <f>AVERAGE(AC3:AC7)</f>
-        <v>6.4000000000000001E-2</v>
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>